<commit_message>
Add better missingness handling; normal lab and vs values
</commit_message>
<xml_diff>
--- a/EDA/table1_pairs.xlsx
+++ b/EDA/table1_pairs.xlsx
@@ -900,31 +900,31 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3870</v>
+        <v>0</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>121 (27.1)</t>
+          <t>121 (21.1)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>127 (12.5)</t>
+          <t>127 (9.3)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>47 (9.5)</t>
+          <t>47 (7.4)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>431 (14.5)</t>
+          <t>431 (11.5)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>1886 (16.8)</t>
+          <t>1886 (13.8)</t>
         </is>
       </c>
     </row>
@@ -938,27 +938,27 @@
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>39 (8.7)</t>
+          <t>39 (6.8)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>94 (9.2)</t>
+          <t>94 (6.9)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>62 (12.5)</t>
+          <t>62 (9.7)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>287 (9.7)</t>
+          <t>287 (7.6)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1529 (13.6)</t>
+          <t>1529 (11.2)</t>
         </is>
       </c>
     </row>
@@ -972,27 +972,27 @@
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>19 (4.3)</t>
+          <t>19 (3.3)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>52 (5.1)</t>
+          <t>52 (3.8)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>23 (4.6)</t>
+          <t>23 (3.6)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>156 (5.3)</t>
+          <t>156 (4.2)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>709 (6.3)</t>
+          <t>709 (5.2)</t>
         </is>
       </c>
     </row>
@@ -1006,27 +1006,27 @@
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>268 (60.0)</t>
+          <t>394 (68.8)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>745 (73.2)</t>
+          <t>1092 (80.0)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>363 (73.3)</t>
+          <t>507 (79.3)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2095 (70.6)</t>
+          <t>2883 (76.7)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>7112 (63.3)</t>
+          <t>9577 (69.9)</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>6 (0.1)</t>
+          <t>6 (0.0)</t>
         </is>
       </c>
     </row>

</xml_diff>